<commit_message>
player and team editing function optimized
</commit_message>
<xml_diff>
--- a/team_data/Sunrisers_SriLanka/Sunrisers_SriLanka.xlsx
+++ b/team_data/Sunrisers_SriLanka/Sunrisers_SriLanka.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\team_data\Sunrisers_SriLanka\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4E9993-ABAE-4173-98F5-7351842E1C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6810" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -79,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +137,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -197,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,27 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,24 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,16 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -523,7 +471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -543,7 +491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -563,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -583,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -603,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -623,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -643,7 +591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -663,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -683,7 +631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -703,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>16</v>
       </c>

</xml_diff>